<commit_message>
refactor workflows, agregar archivos a solfacs
</commit_message>
<xml_diff>
--- a/Backend/src/Sofco.WebApi/wwwroot/excelTemplates/remito.xlsx
+++ b/Backend/src/Sofco.WebApi/wwwroot/excelTemplates/remito.xlsx
@@ -58,7 +58,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="FrutigerRoman"/>
@@ -96,44 +96,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -158,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -245,11 +209,11 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -260,57 +224,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -621,7 +543,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D13" sqref="D13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1"/>
@@ -688,7 +610,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="39"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:13">
@@ -755,11 +677,11 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
       <c r="I10" s="5"/>
       <c r="J10" s="11"/>
     </row>
@@ -767,11 +689,11 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="30"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="13"/>
       <c r="I11" s="5"/>
       <c r="J11" s="11"/>
     </row>
@@ -779,11 +701,11 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="30"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="5"/>
       <c r="J12" s="11"/>
     </row>
@@ -791,11 +713,11 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="5"/>
       <c r="J13" s="11"/>
     </row>
@@ -843,7 +765,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -891,7 +813,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="31"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
@@ -926,24 +848,24 @@
     <row r="24" spans="1:10">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="5"/>
     </row>
@@ -951,7 +873,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="14"/>
-      <c r="D26" s="36"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="21"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -966,7 +888,7 @@
       <c r="D27" s="20"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="33"/>
+      <c r="G27" s="15"/>
       <c r="H27" s="22"/>
       <c r="I27" s="23"/>
       <c r="J27" s="8"/>
@@ -987,7 +909,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="14"/>
-      <c r="D29" s="37"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -999,7 +921,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="38"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1011,7 +933,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="38"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -1023,7 +945,7 @@
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="38"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -1035,7 +957,7 @@
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="38"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -1047,7 +969,7 @@
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="14"/>
-      <c r="D34" s="38"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1059,7 +981,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="14"/>
-      <c r="D35" s="34"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -1071,7 +993,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="14"/>
-      <c r="D36" s="35"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -1083,7 +1005,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="35"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="24"/>
@@ -1095,7 +1017,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="5"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="35"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -1107,7 +1029,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="5"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="35"/>
+      <c r="D39" s="15"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -1292,16 +1214,14 @@
     </row>
   </sheetData>
   <sheetProtection password="83AF" sheet="1" objects="1" scenarios="1" formatCells="0" selectLockedCells="1"/>
-  <mergeCells count="6">
-    <mergeCell ref="D25:H25"/>
+  <mergeCells count="4">
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D24:H24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10:J14">
       <formula1>"x"</formula1>
     </dataValidation>
@@ -1387,7 +1307,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="4">
         <f ca="1">TODAY()</f>
-        <v>42983</v>
+        <v>43000</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -1455,11 +1375,11 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="5"/>
       <c r="J10" s="11"/>
     </row>
@@ -1467,10 +1387,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="13"/>
       <c r="I11" s="5"/>
       <c r="J11" s="11"/>
@@ -1479,10 +1399,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="13"/>
       <c r="I12" s="5"/>
       <c r="J12" s="11"/>
@@ -1491,11 +1411,11 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="5"/>
       <c r="J13" s="11"/>
     </row>
@@ -2084,7 +2004,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="4">
         <f ca="1">TODAY()</f>
-        <v>42983</v>
+        <v>43000</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -2152,11 +2072,11 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="5"/>
       <c r="J10" s="11"/>
     </row>
@@ -2164,10 +2084,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="13"/>
       <c r="I11" s="5"/>
       <c r="J11" s="11"/>
@@ -2176,10 +2096,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="13"/>
       <c r="I12" s="5"/>
       <c r="J12" s="11"/>
@@ -2188,11 +2108,11 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="5"/>
       <c r="J13" s="11"/>
     </row>
@@ -2781,7 +2701,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="4">
         <f ca="1">TODAY()</f>
-        <v>42983</v>
+        <v>43000</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -2849,11 +2769,11 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="5"/>
       <c r="J10" s="11"/>
     </row>
@@ -2861,10 +2781,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="13"/>
       <c r="I11" s="5"/>
       <c r="J11" s="11"/>
@@ -2873,10 +2793,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="13"/>
       <c r="I12" s="5"/>
       <c r="J12" s="11"/>
@@ -2885,11 +2805,11 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="5"/>
       <c r="J13" s="11"/>
     </row>
@@ -3405,33 +3325,128 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Remito" ma:contentTypeID="0x010100C4D9C75A9CAEC34AA1E778E9D444C32900B4EBC0AECE543C47B8BC4617E12A365D" ma:contentTypeVersion="6" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="274740f43e8fb25279531480f506914c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="045c21bd28c8aa822ee924ae5ab52af2">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005918CC9680C2504181E2B8642301C8C3" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="32a846daf22536a6bbc872f5aa924d77">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cdb0fcb8-ece9-4a71-82df-3727f0966003" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e17f1d673cef6e7fe6316a179d930a6" ns2:_="">
+    <xsd:import namespace="cdb0fcb8-ece9-4a71-82df-3727f0966003"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
-              <xsd:all/>
+              <xsd:all>
+                <xsd:element ref="ns2:Proceso" minOccurs="0"/>
+                <xsd:element ref="ns2:tipodedocumento" minOccurs="0"/>
+                <xsd:element ref="ns2:Sector_x0020_Responsable_x0020_Archivo" minOccurs="0"/>
+                <xsd:element ref="ns2:Medio_x0020_almacenamiento" minOccurs="0"/>
+                <xsd:element ref="ns2:Tiempo_x0020_minimo_x0020_archivo" minOccurs="0"/>
+                <xsd:element ref="ns2:Norma_x0020_ISO" minOccurs="0"/>
+                <xsd:element ref="ns2:Modelo_x0020_CMMI_x0020_DEV" minOccurs="0"/>
+                <xsd:element ref="ns2:Modelo_x0020_CMMI_x0020_SVC" minOccurs="0"/>
+                <xsd:element ref="ns2:SOX_x0020__x0028_Sede_x0029_" minOccurs="0"/>
+              </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cdb0fcb8-ece9-4a71-82df-3727f0966003" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Proceso" ma:index="2" nillable="true" ma:displayName="Proceso" ma:default="CM" ma:description="Proceso" ma:format="Dropdown" ma:internalName="Proceso">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="CG"/>
+          <xsd:enumeration value="CM"/>
+          <xsd:enumeration value="COMP"/>
+          <xsd:enumeration value="DAR"/>
+          <xsd:enumeration value="DD"/>
+          <xsd:enumeration value="ET"/>
+          <xsd:enumeration value="GAF"/>
+          <xsd:enumeration value="GE"/>
+          <xsd:enumeration value="IT"/>
+          <xsd:enumeration value="MA"/>
+          <xsd:enumeration value="OPM"/>
+          <xsd:enumeration value="OT"/>
+          <xsd:enumeration value="OTROS"/>
+          <xsd:enumeration value="PE"/>
+          <xsd:enumeration value="PMC"/>
+          <xsd:enumeration value="PP"/>
+          <xsd:enumeration value="PPQA"/>
+          <xsd:enumeration value="PROV"/>
+          <xsd:enumeration value="RE"/>
+          <xsd:enumeration value="REQM"/>
+          <xsd:enumeration value="RPP"/>
+          <xsd:enumeration value="SAM"/>
+          <xsd:enumeration value="SCON"/>
+          <xsd:enumeration value="TST"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="tipodedocumento" ma:index="3" nillable="true" ma:displayName="Tipo de Documento" ma:default="Chequeo" ma:description="Tipo de Documento" ma:format="Dropdown" ma:internalName="tipodedocumento">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Chequeo"/>
+          <xsd:enumeration value="Formulario"/>
+          <xsd:enumeration value="Guía"/>
+          <xsd:enumeration value="Imágenes"/>
+          <xsd:enumeration value="Marcos de Proceso"/>
+          <xsd:enumeration value="Proceso"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Sector_x0020_Responsable_x0020_Archivo" ma:index="4" nillable="true" ma:displayName="Sector Responsable Archivo" ma:description="Sector Responsable Archivo" ma:internalName="Sector_x0020_Responsable_x0020_Archivo">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Medio_x0020_almacenamiento" ma:index="5" nillable="true" ma:displayName="Medio almacenamiento" ma:default="" ma:description="Medio almacenamiento" ma:internalName="Medio_x0020_almacenamiento">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Tiempo_x0020_minimo_x0020_archivo" ma:index="6" nillable="true" ma:displayName="Tiempo minimo archivo" ma:description="Tiempo minimo archivo" ma:internalName="Tiempo_x0020_minimo_x0020_archivo">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Norma_x0020_ISO" ma:index="15" nillable="true" ma:displayName="Norma ISO" ma:internalName="Norma_x0020_ISO">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Modelo_x0020_CMMI_x0020_DEV" ma:index="16" nillable="true" ma:displayName="Modelo CMMI DEV" ma:internalName="Modelo_x0020_CMMI_x0020_DEV">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Modelo_x0020_CMMI_x0020_SVC" ma:index="17" nillable="true" ma:displayName="Modelo CMMI SVC" ma:internalName="Modelo_x0020_CMMI_x0020_SVC">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SOX_x0020__x0028_Sede_x0029_" ma:index="18" nillable="true" ma:displayName="SOX (Sede)" ma:internalName="SOX_x0020__x0028_Sede_x0029_">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -3443,8 +3458,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="10" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -3533,47 +3548,77 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Tiempo_x0020_minimo_x0020_archivo xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003">10 años</Tiempo_x0020_minimo_x0020_archivo>
+    <tipodedocumento xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003">Formulario</tipodedocumento>
+    <Modelo_x0020_CMMI_x0020_SVC xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003" xsi:nil="true"/>
+    <Medio_x0020_almacenamiento xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003">Digital</Medio_x0020_almacenamiento>
+    <Norma_x0020_ISO xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003" xsi:nil="true"/>
+    <SOX_x0020__x0028_Sede_x0029_ xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003" xsi:nil="true"/>
+    <Sector_x0020_Responsable_x0020_Archivo xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003">Operaciones</Sector_x0020_Responsable_x0020_Archivo>
+    <Proceso xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003">PMC</Proceso>
+    <Modelo_x0020_CMMI_x0020_DEV xmlns="cdb0fcb8-ece9-4a71-82df-3727f0966003" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635D69BF-AF4D-44C9-93E2-83B2322AB8C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5368229-04D4-40FE-8CE7-5B9F5E5B9165}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cdb0fcb8-ece9-4a71-82df-3727f0966003"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A4595A-772D-4406-B7C5-78DA76632FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="cdb0fcb8-ece9-4a71-82df-3727f0966003"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD20D4F2-46CE-4AF2-B0BD-36B0E46FAA6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE681AA9-C65E-402F-9800-F524456D7DB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4838562F-AC29-4033-B619-AA1B86DBC2FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635D69BF-AF4D-44C9-93E2-83B2322AB8C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>